<commit_message>
RTL Updates:    -implemented DCO module, created automatic calculator for the DCO and registers    -implemented PWM module    -discovered bugs in Timer and PWM modules regarding HW updates on slower clocks( will fix in next revision)    -small updates to the timer    -added new registers types to the sfr pkg
</commit_message>
<xml_diff>
--- a/RTL/Timer/Timer Registers.xlsx
+++ b/RTL/Timer/Timer Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211D8FED-73C7-4CC7-80DD-3060B5C58E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256C17B3-515D-4BEE-93D5-8D49E7321575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{C2F59BC8-B028-4C30-AFB2-8B1588A6E92D}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="8775" windowHeight="11385" xr2:uid="{C2F59BC8-B028-4C30-AFB2-8B1588A6E92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="135">
   <si>
     <t>Timer registers</t>
   </si>
@@ -185,9 +185,6 @@
     <t>TVAL[0]</t>
   </si>
   <si>
-    <t>TMCH[15]</t>
-  </si>
-  <si>
     <t>CLKSRC[0]</t>
   </si>
   <si>
@@ -432,6 +429,18 @@
   </si>
   <si>
     <t>R/W/HS/HC</t>
+  </si>
+  <si>
+    <t>TMCH1[15]</t>
+  </si>
+  <si>
+    <t>MATCH1_EN</t>
+  </si>
+  <si>
+    <t>MATCH0_EN</t>
+  </si>
+  <si>
+    <t>OVF_EN</t>
   </si>
 </sst>
 </file>
@@ -833,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3234D1-D8E4-42D2-A322-A69FD8618541}">
   <dimension ref="B2:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,18 +900,18 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -996,13 +1005,13 @@
     </row>
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>2</v>
@@ -1021,9 +1030,15 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1075,13 +1090,13 @@
     </row>
     <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>2</v>
@@ -1101,24 +1116,24 @@
     </row>
     <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1166,10 +1181,10 @@
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>2</v>
@@ -1178,13 +1193,13 @@
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>16</v>
@@ -1192,21 +1207,21 @@
     </row>
     <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>13</v>
@@ -1252,28 +1267,28 @@
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1347,28 +1362,28 @@
     </row>
     <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1442,28 +1457,28 @@
     </row>
     <row r="42" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1537,28 +1552,28 @@
     </row>
     <row r="46" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1622,7 +1637,7 @@
     </row>
     <row r="53" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1653,28 +1668,28 @@
     </row>
     <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1748,28 +1763,28 @@
     </row>
     <row r="59" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1843,28 +1858,28 @@
     </row>
     <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1938,28 +1953,28 @@
     </row>
     <row r="67" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1997,7 +2012,7 @@
     </row>
     <row r="73" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2028,28 +2043,28 @@
     </row>
     <row r="75" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="76" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2123,28 +2138,28 @@
     </row>
     <row r="79" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="80" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2218,28 +2233,28 @@
     </row>
     <row r="83" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2313,28 +2328,28 @@
     </row>
     <row r="87" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>